<commit_message>
Yet more file structure changes + DB Setup
If DB doesn't exist, creates one as well as the table with required shema.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C45CDBD-AF33-484B-949F-19C44D4A8A41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0F8E52-BD34-48F5-B74F-48668DDF46B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Phase 1</t>
   </si>
@@ -80,15 +80,9 @@
     <t xml:space="preserve">Admin call </t>
   </si>
   <si>
-    <t>Attendance stats</t>
-  </si>
-  <si>
     <t>Table created</t>
   </si>
   <si>
-    <t>Test schedule</t>
-  </si>
-  <si>
     <t>Credentials:</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
     <t>Admin promotion/demotion</t>
   </si>
   <si>
-    <t>DB Schema</t>
-  </si>
-  <si>
     <t>NickName</t>
   </si>
   <si>
@@ -192,13 +183,70 @@
   </si>
   <si>
     <t>check when someone signs but doesn't turn up</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>Query Nicknames based on ID? When?</t>
+  </si>
+  <si>
+    <t>Find a place to query nickname based on Id</t>
+  </si>
+  <si>
+    <t>Add user into table command - catch bad commands</t>
+  </si>
+  <si>
+    <t>Attendance stats - monthly report?</t>
+  </si>
+  <si>
+    <t>Test schedule - catches properly</t>
+  </si>
+  <si>
+    <t>View Table Data</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">select * from </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'TableName'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> limit X</t>
+    </r>
+  </si>
+  <si>
+    <t>DB Schema - InitialTestTable - InitialTestDB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +272,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -615,15 +671,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
@@ -678,231 +734,259 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>49</v>
+    <row r="27" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="B39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="5" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C36" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>5.7852753265636096E+17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>5.7852753265636096E+17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B50" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
+      <c r="A52" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-    </row>
-    <row r="54" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A53" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>53</v>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B36" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
-    <hyperlink ref="B37" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
+    <hyperlink ref="B38" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
+    <hyperlink ref="B39" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Add and Wipe Command Added
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0F8E52-BD34-48F5-B74F-48668DDF46B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AC4CDA-EB20-4B03-B3DE-E312CE952181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Phase 1</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Messages between bot and server</t>
-  </si>
-  <si>
-    <t>GET and POST</t>
   </si>
   <si>
     <t xml:space="preserve">Admin call </t>
@@ -240,6 +237,48 @@
   </si>
   <si>
     <t>DB Schema - InitialTestTable - InitialTestDB</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Bot Command Prefix</t>
+  </si>
+  <si>
+    <t>Error returns and suggestions</t>
+  </si>
+  <si>
+    <t>DiscId</t>
+  </si>
+  <si>
+    <t>Structure will break if rank has a space</t>
+  </si>
+  <si>
+    <t>Send picture for sign/unsign?</t>
+  </si>
+  <si>
+    <t>Check if Id is a member of the server when adding</t>
+  </si>
+  <si>
+    <t>Maybe take out wipe for release</t>
+  </si>
+  <si>
+    <t>Take our hardcoded references. E.g. channels and guilds etc</t>
+  </si>
+  <si>
+    <t>BobbleHat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don’t think I need a nickname  - &lt;@ID&gt; will </t>
+  </si>
+  <si>
+    <t>Remind system? Mention 36 hours before.</t>
+  </si>
+  <si>
+    <t>Add horrendous picture send for tom sign.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make sure its only PMs that the bot picks up </t>
   </si>
 </sst>
 </file>
@@ -671,15 +710,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
@@ -733,13 +772,13 @@
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
+      <c r="A12" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -754,7 +793,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -764,27 +803,27 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -794,7 +833,7 @@
     </row>
     <row r="27" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -804,92 +843,92 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
         <v>43</v>
       </c>
-      <c r="B35" t="s">
-        <v>44</v>
-      </c>
       <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" t="s">
         <v>40</v>
       </c>
-      <c r="D35" t="s">
-        <v>41</v>
-      </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" t="s">
-        <v>21</v>
-      </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -899,88 +938,167 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="B51" t="s">
         <v>33</v>
       </c>
-      <c r="B51" t="s">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="B52" t="s">
         <v>35</v>
       </c>
-      <c r="B52" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="B53" t="s">
         <v>37</v>
       </c>
-      <c r="B53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="10"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>52</v>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed to Promise-based function rather than callback.
I've done this because "returning" out of a callback is a PITA and the previous setup had order of execution issues and I didn't want to just use timeouts until async callbacks had executed.
Also moved most channel.sends to the MessageHandler because as mentioned, returning a string from the function call with async methods are very annoying. Much easier to just pass the channel as a parameter into the function itself and calling it from there.
Further housekeeping as well, syntax errors, if condition refactoring etc etc.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AC4CDA-EB20-4B03-B3DE-E312CE952181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1EA82A-05D9-4376-9E7F-22DA7591897E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>Phase 1</t>
   </si>
@@ -279,6 +279,21 @@
   </si>
   <si>
     <t xml:space="preserve">make sure its only PMs that the bot picks up </t>
+  </si>
+  <si>
+    <t>Confirmation mechanic? By role?</t>
+  </si>
+  <si>
+    <t>Bobblehat</t>
+  </si>
+  <si>
+    <t>BobbleHat is causing a warning in the log</t>
+  </si>
+  <si>
+    <t>I'm worried about thread safety.</t>
+  </si>
+  <si>
+    <t>Remove (demote to social?)</t>
   </si>
 </sst>
 </file>
@@ -381,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -395,6 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -710,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,8 +793,13 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -823,47 +844,50 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>42</v>
       </c>
       <c r="B35" t="s">
         <v>43</v>
@@ -881,14 +905,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>19</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>21</v>
@@ -902,7 +926,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>22</v>
@@ -913,48 +937,50 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>5.7852753265636096E+17</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="B48" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="B51" t="s">
         <v>33</v>
@@ -962,7 +988,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B52" t="s">
         <v>35</v>
@@ -970,42 +996,42 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
+      <c r="A54" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-    </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="10"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="B59" s="10"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>62</v>
@@ -1018,87 +1044,107 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
+      <c r="A61" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
+      <c r="A63" s="10"/>
     </row>
     <row r="64" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving commands into their own script file
Means I don't have a MessageHandler class a mile long and navigation to command behaviour is easier.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1EA82A-05D9-4376-9E7F-22DA7591897E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AC9A68-A2E5-45C5-ACC6-9E99D6D519BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>Phase 1</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Database querying return</t>
-  </si>
-  <si>
-    <t>Messages between bot and server</t>
   </si>
   <si>
     <t xml:space="preserve">Admin call </t>
@@ -287,13 +284,22 @@
     <t>Bobblehat</t>
   </si>
   <si>
-    <t>BobbleHat is causing a warning in the log</t>
-  </si>
-  <si>
     <t>I'm worried about thread safety.</t>
   </si>
   <si>
     <t>Remove (demote to social?)</t>
+  </si>
+  <si>
+    <t>Add startup test data - manual insert disc Id</t>
+  </si>
+  <si>
+    <t>User wipe all signs</t>
+  </si>
+  <si>
+    <t>User sign for month?</t>
+  </si>
+  <si>
+    <t>Move commands into their own script files.</t>
   </si>
 </sst>
 </file>
@@ -408,9 +414,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -726,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,52 +795,52 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -844,25 +850,27 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-    </row>
-    <row r="27" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>44</v>
+      <c r="A28" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -872,92 +880,92 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
         <v>39</v>
       </c>
-      <c r="D35" t="s">
-        <v>40</v>
-      </c>
       <c r="E35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" t="s">
-        <v>20</v>
+      <c r="D39" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,12 +975,12 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -980,31 +988,31 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1012,12 +1020,12 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1025,27 +1033,27 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="10"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,98 +1067,103 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B38" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
-    <hyperlink ref="B39" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
+    <hyperlink ref="B39" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
+    <hyperlink ref="B40" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Promotion functionality entered and Promise source moved to it's own file
It would have got a bit annoying to have to put Promise functionality for queries in all the commands that interact with the database. for the sake of one line of require code, its definitely worth it.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AC9A68-A2E5-45C5-ACC6-9E99D6D519BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD3E6C-2165-4289-9984-52F8A6783D6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
   <si>
     <t>Phase 1</t>
   </si>
@@ -143,9 +143,6 @@
     <t>DB Admin</t>
   </si>
   <si>
-    <t>Admin promotion/demotion</t>
-  </si>
-  <si>
     <t>NickName</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
   </si>
   <si>
     <t>Query Nicknames based on ID? When?</t>
-  </si>
-  <si>
-    <t>Find a place to query nickname based on Id</t>
   </si>
   <si>
     <t>Add user into table command - catch bad commands</t>
@@ -299,7 +293,37 @@
     <t>User sign for month?</t>
   </si>
   <si>
-    <t>Move commands into their own script files.</t>
+    <t>Move commands into own script file</t>
+  </si>
+  <si>
+    <t>when this goes live, hardcode admin user to promote officers off the bat</t>
+  </si>
+  <si>
+    <t>Find a place to query nickname based on Id - or just use &lt;@...&gt; in mentions?</t>
+  </si>
+  <si>
+    <t>Admin promotion/demotion/Delete</t>
+  </si>
+  <si>
+    <t>permissions - only officers can edit other users</t>
+  </si>
+  <si>
+    <t>Promote/Demote</t>
+  </si>
+  <si>
+    <t>Rename function</t>
+  </si>
+  <si>
+    <t>Don't allow the same nickname in DB</t>
+  </si>
+  <si>
+    <t>Do I need so many returns?</t>
+  </si>
+  <si>
+    <t>Hard coded table/db names?</t>
+  </si>
+  <si>
+    <t>Admin check rank command</t>
   </si>
 </sst>
 </file>
@@ -732,15 +756,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
@@ -800,52 +824,50 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A15" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+    </row>
+    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -855,217 +877,230 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>44</v>
+      <c r="A30" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
         <v>38</v>
       </c>
-      <c r="D35" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="B48">
         <v>5.7852753265636096E+17</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-    </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B51" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="A56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>56</v>
+      <c r="A57" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
+      <c r="A58" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="10"/>
+      <c r="A59" s="10"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" t="s">
-        <v>39</v>
-      </c>
-      <c r="D60" t="s">
-        <v>38</v>
-      </c>
+      <c r="A60" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="10"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
+      <c r="A62" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-    </row>
-    <row r="64" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+    </row>
+    <row r="65" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>25</v>
       </c>
@@ -1075,95 +1110,130 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B39" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
-    <hyperlink ref="B40" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
+    <hyperlink ref="B41" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
+    <hyperlink ref="B42" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Shift towards google sheets
The output from a straight up DB seems like it would be a gigantic pain and also not visually engaging. Interacting from discord to a google sheet should provide a much better link for the user. Remains to be seen whether a db is even required.

More importantly, moved auth credentials into a gitignored json file.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C64BEE-3247-4E2F-99F5-CBD83D33CB8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A12DD4-48FB-45B3-A6DE-8B39ABA4EBB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
   <si>
     <t>Phase 1</t>
   </si>
@@ -333,6 +333,24 @@
   </si>
   <si>
     <t>Make sure all queries limit one user, just in case</t>
+  </si>
+  <si>
+    <t>SQL injection protection</t>
+  </si>
+  <si>
+    <t>Ranks are held in Disc already</t>
+  </si>
+  <si>
+    <t>ask offs about visibility</t>
+  </si>
+  <si>
+    <t>Shift google dot by one every day at…. Urrrr 4:30am?</t>
+  </si>
+  <si>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t>get spreadsheet rolling by date</t>
   </si>
 </sst>
 </file>
@@ -435,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -449,6 +467,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -764,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,8 +795,7 @@
     <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1118,139 +1137,165 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="C68" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed authing and initial interaction with google doc.
Also put in unfinished functionality that gets date objects for the next 8 weeks.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AFCC71-F9E4-4E2A-A7BB-34B236E7C691}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD9CD15-B84D-436D-A795-3F4006FF6E20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
   <si>
     <t>Phase 1</t>
   </si>
@@ -351,6 +351,15 @@
   </si>
   <si>
     <t>get spreadsheet rolling by date</t>
+  </si>
+  <si>
+    <t>Google Doc</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/19zU2Dz78yuttROuU0z54j2S2Fy2gG_gthiE5qrLqsYU/edit#gid=0</t>
+  </si>
+  <si>
+    <t>Clean up consts and dependencies</t>
   </si>
 </sst>
 </file>
@@ -453,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -469,6 +478,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -784,15 +794,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="5" width="30" customWidth="1"/>
@@ -1007,303 +1017,320 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>23</v>
+      <c r="A44" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B46">
+      <c r="B49">
         <v>5.7852753265636096E+17</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B55" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="B56" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
+      <c r="A57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="10"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" t="s">
-        <v>37</v>
-      </c>
-      <c r="D59" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" t="s">
-        <v>37</v>
-      </c>
-      <c r="D60" t="s">
-        <v>36</v>
-      </c>
+      <c r="A60" s="10"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" t="s">
-        <v>36</v>
-      </c>
+      <c r="A61" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" s="10"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-    </row>
-    <row r="64" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+    </row>
+    <row r="67" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+    <row r="68" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>48</v>
+        <v>26</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D72" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B39" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
     <hyperlink ref="B40" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
+    <hyperlink ref="A44" r:id="rId3" location="gid=0" display="https://docs.google.com/spreadsheets/d/19zU2Dz78yuttROuU0z54j2S2Fy2gG_gthiE5qrLqsYU/edit - gid=0" xr:uid="{8765783E-5E2E-4619-A5C8-CBED2CD262B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update and Spreadsheet input
Preliminary google sheet interaction
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD9CD15-B84D-436D-A795-3F4006FF6E20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC420DA-194E-4BA3-B340-C6F7D039826C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
   <si>
     <t>Phase 1</t>
   </si>
@@ -360,6 +360,39 @@
   </si>
   <si>
     <t>Clean up consts and dependencies</t>
+  </si>
+  <si>
+    <t>Crash protection - maybe use the DB?</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Lemon</t>
+  </si>
+  <si>
+    <t>populate user sheet by role on reset</t>
+  </si>
+  <si>
+    <t>https://github.com/theoephraim/node-google-spreadsheet/compare/master...reptily:patch-1</t>
+  </si>
+  <si>
+    <t>FUCK IT! I GIVE UP. Let the admins add more columns and just search for the date keys for inserts</t>
+  </si>
+  <si>
+    <t>Do I need promises</t>
+  </si>
+  <si>
+    <t>take out dbconnect if not using</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 -&gt; 05 June user input </t>
+  </si>
+  <si>
+    <t>for now, im disabling screen population on startup. Debugging takes too long. Also investigate when it sometimes doesn't populate the dates correctly</t>
+  </si>
+  <si>
+    <t>The start screen dates seem all our of whack</t>
   </si>
 </sst>
 </file>
@@ -794,10 +827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
-  <dimension ref="A1:F100"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,72 +843,78 @@
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1324,13 +1364,62 @@
         <v>99</v>
       </c>
     </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B39" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
     <hyperlink ref="B40" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
-    <hyperlink ref="A44" r:id="rId3" location="gid=0" display="https://docs.google.com/spreadsheets/d/19zU2Dz78yuttROuU0z54j2S2Fy2gG_gthiE5qrLqsYU/edit - gid=0" xr:uid="{8765783E-5E2E-4619-A5C8-CBED2CD262B2}"/>
+    <hyperlink ref="A44" r:id="rId3" location="gid=0" xr:uid="{8765783E-5E2E-4619-A5C8-CBED2CD262B2}"/>
+    <hyperlink ref="A103" r:id="rId4" xr:uid="{42259F3D-42D3-4505-A85E-BF9078FD1266}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Historic data preservation functionality
functionality for preserving past dates, curiously.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07EF476-1CFA-447C-B9FD-13F22C830EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65426D16-6F40-4C6C-91B1-E853BAE6CDB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="88">
   <si>
     <t>Phase 1</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>S4Month</t>
+  </si>
+  <si>
+    <t>Deprecated code clean up</t>
+  </si>
+  <si>
+    <t>Theres going to be some funky overflows in the new year</t>
+  </si>
+  <si>
+    <t>sign Wed 05 Jub is accepted but doesn't do anything.  Mispelt month names and incorrect day values. E.g. the 234th of May</t>
+  </si>
+  <si>
+    <t>Can't change confirmed to attending (NA is fine)</t>
   </si>
 </sst>
 </file>
@@ -747,10 +759,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9571B65A-1634-40DF-8B4F-4BFD915E6E44}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,14 +844,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -847,204 +859,195 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="20" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>32</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>33</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>37</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>5.7852753265636096E+17</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-    </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-    </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="10"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="10"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C55" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" t="s">
-        <v>32</v>
-      </c>
+      <c r="B55" s="10"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>46</v>
@@ -1058,151 +1061,175 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-    </row>
-    <row r="60" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
+      <c r="A59" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+    </row>
+    <row r="61" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>47</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D63" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B32" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
-    <hyperlink ref="B33" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
-    <hyperlink ref="A37" r:id="rId3" location="gid=0" xr:uid="{8765783E-5E2E-4619-A5C8-CBED2CD262B2}"/>
-    <hyperlink ref="A74" r:id="rId4" xr:uid="{42259F3D-42D3-4505-A85E-BF9078FD1266}"/>
+    <hyperlink ref="B33" r:id="rId1" xr:uid="{D06990C0-4D86-4C25-9A72-D4F1670267CE}"/>
+    <hyperlink ref="B34" r:id="rId2" xr:uid="{01CD3419-367E-454B-BCD8-210246DDBF13}"/>
+    <hyperlink ref="A38" r:id="rId3" location="gid=0" xr:uid="{8765783E-5E2E-4619-A5C8-CBED2CD262B2}"/>
+    <hyperlink ref="A75" r:id="rId4" xr:uid="{42259F3D-42D3-4505-A85E-BF9078FD1266}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Tom functionality, just because it makes me giggle.
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SLM-Sign-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F415FD2-7633-4CA4-B9BC-E642D9302DA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B1C79A-4672-4CA3-AC37-E0316CCBBB8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AA72A287-1B54-4516-B2F4-E7652AD4D042}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
   <si>
     <t>Phase 1</t>
   </si>
@@ -194,21 +194,9 @@
     <t>DB Schema - InitialTestTable - InitialTestDB</t>
   </si>
   <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>Bot Command Prefix</t>
-  </si>
-  <si>
-    <t>DiscId</t>
-  </si>
-  <si>
     <t>Take our hardcoded references. E.g. channels and guilds etc</t>
   </si>
   <si>
-    <t>BobbleHat</t>
-  </si>
-  <si>
     <t>Add horrendous picture send for tom sign.</t>
   </si>
   <si>
@@ -227,9 +215,6 @@
     <t>permissions - only officers can edit other users</t>
   </si>
   <si>
-    <t>Promote/Demote</t>
-  </si>
-  <si>
     <t>Do I need so many returns?</t>
   </si>
   <si>
@@ -237,15 +222,6 @@
   </si>
   <si>
     <t>Make sure plebs can't message the bot</t>
-  </si>
-  <si>
-    <t>Kick</t>
-  </si>
-  <si>
-    <t>TODO:</t>
-  </si>
-  <si>
-    <t>get spreadsheet rolling by date</t>
   </si>
   <si>
     <t>Google Doc</t>
@@ -758,8 +734,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,12 +799,12 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -838,22 +814,22 @@
     </row>
     <row r="16" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -869,12 +845,12 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,12 +860,12 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -954,12 +930,12 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1004,7 +980,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>28</v>
       </c>
@@ -1012,7 +988,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>30</v>
       </c>
@@ -1020,205 +996,172 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="10"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C56" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="B55" s="10">
+        <v>1.97684665757204E+17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
     </row>
-    <row r="61" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D64" t="s">
-        <v>61</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C64" s="4"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>